<commit_message>
Update RN1 in Remote BOM, Update Readme, add link to Wiki for mods
</commit_message>
<xml_diff>
--- a/PCB_files/IC905_Remote_BCD_Band_Decoder_PCB_V1.1/Remote BCD_Decoder_BOM_31-Jan-2025_V1.1.xlsx
+++ b/PCB_files/IC905_Remote_BCD_Band_Decoder_PCB_V1.1/Remote BCD_Decoder_BOM_31-Jan-2025_V1.1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{65B32AEF-724B-4148-B9DF-9BC429EFC9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51B217C9-EA24-46DC-8588-1DDA0912C9E5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEDEEB9-DD4C-4288-82FC-498D0BE90DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="795" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="2925" windowWidth="21600" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Remote Demux Board_Demux_Bo" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="123">
   <si>
     <t>No.</t>
   </si>
@@ -185,9 +185,6 @@
     <t>10 pos plug</t>
   </si>
   <si>
-    <t>8x1KΩ</t>
-  </si>
-  <si>
     <t>5.0V</t>
   </si>
   <si>
@@ -299,18 +296,6 @@
     <t>Bourns Inc.</t>
   </si>
   <si>
-    <t>4609X-101-102LF</t>
-  </si>
-  <si>
-    <t>4609X-101-102LF-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/bourns-inc/4609X-101-102LF/3593658</t>
-  </si>
-  <si>
-    <t>RES ARRAY 8 RES 1K OHM 9SIP</t>
-  </si>
-  <si>
     <t>13-CFR-25JR-52-330RCT-ND</t>
   </si>
   <si>
@@ -384,6 +369,21 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/eaton-electronics-division/PTR030V0110-BK/2675229</t>
+  </si>
+  <si>
+    <t>RES ARRAY 8 RES 220 OHM 9SIP</t>
+  </si>
+  <si>
+    <t>8x220Ω</t>
+  </si>
+  <si>
+    <t>4609X-101-221LF</t>
+  </si>
+  <si>
+    <t>4609X-101-221LF-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/4609X-101-221LF/3593660</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -438,6 +438,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -781,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +841,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -844,16 +850,16 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -864,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -873,16 +879,16 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -893,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -902,16 +908,16 @@
         <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -922,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
@@ -931,16 +937,16 @@
         <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -951,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
@@ -960,16 +966,16 @@
         <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -980,25 +986,25 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="I7" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1009,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
@@ -1018,16 +1024,16 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1053,10 +1059,10 @@
         <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1067,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>47</v>
@@ -1082,10 +1088,10 @@
         <v>46</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1096,7 +1102,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
@@ -1111,10 +1117,10 @@
         <v>46</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1125,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>48</v>
@@ -1154,25 +1160,25 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1192,16 +1198,16 @@
         <v>51</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1212,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>34</v>
@@ -1221,45 +1227,45 @@
         <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>96</v>
+      <c r="E16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1270,7 +1276,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>37</v>
@@ -1279,14 +1285,14 @@
         <v>17</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1297,7 +1303,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>40</v>
@@ -1309,13 +1315,13 @@
         <v>39</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1332,7 +1338,7 @@
         <v>43</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>42</v>
@@ -1363,13 +1369,13 @@
     <hyperlink ref="I5" r:id="rId5" xr:uid="{B2A231AB-F36C-4E66-A076-054BA39C3D04}"/>
     <hyperlink ref="I4" r:id="rId6" xr:uid="{F603EE76-9EED-47F7-B22D-B91BFCA2977E}"/>
     <hyperlink ref="I13" r:id="rId7" xr:uid="{273BD2B9-A09D-4094-9F56-A6655DEA6C59}"/>
-    <hyperlink ref="I16" r:id="rId8" xr:uid="{A784BCE2-A2D8-4C8D-9F5C-731FDAE55803}"/>
-    <hyperlink ref="I15" r:id="rId9" display="https://www.digikey.com/en/products/detail/yageo/CFR-25JR-52-330R/11962" xr:uid="{8237DAC6-311C-4ED4-B302-A4B001AA06BA}"/>
-    <hyperlink ref="I18" r:id="rId10" xr:uid="{4D7E58C0-5FE3-4057-A35D-065283EBF2A9}"/>
-    <hyperlink ref="I17" r:id="rId11" xr:uid="{728AA35E-B42B-4455-BDFF-854B96B1F9A0}"/>
-    <hyperlink ref="I6" r:id="rId12" xr:uid="{FE602473-71B1-4A09-B044-305A36042B0C}"/>
-    <hyperlink ref="I3" r:id="rId13" xr:uid="{C7F84057-41D5-4ABB-B419-96509B516BE0}"/>
-    <hyperlink ref="I2" r:id="rId14" xr:uid="{CA4B64A0-43FD-4DC9-9AF3-CEBBB0806805}"/>
+    <hyperlink ref="I15" r:id="rId8" display="https://www.digikey.com/en/products/detail/yageo/CFR-25JR-52-330R/11962" xr:uid="{8237DAC6-311C-4ED4-B302-A4B001AA06BA}"/>
+    <hyperlink ref="I18" r:id="rId9" xr:uid="{4D7E58C0-5FE3-4057-A35D-065283EBF2A9}"/>
+    <hyperlink ref="I17" r:id="rId10" xr:uid="{728AA35E-B42B-4455-BDFF-854B96B1F9A0}"/>
+    <hyperlink ref="I6" r:id="rId11" xr:uid="{FE602473-71B1-4A09-B044-305A36042B0C}"/>
+    <hyperlink ref="I3" r:id="rId12" xr:uid="{C7F84057-41D5-4ABB-B419-96509B516BE0}"/>
+    <hyperlink ref="I2" r:id="rId13" xr:uid="{CA4B64A0-43FD-4DC9-9AF3-CEBBB0806805}"/>
+    <hyperlink ref="I16" r:id="rId14" xr:uid="{3383CBD8-4223-492C-88C3-945580104F9C}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>